<commit_message>
add the function to convert .gjf file to .mol file
just need to use counterA.mole.generateMOLFile() as the test.py file
</commit_message>
<xml_diff>
--- a/demoForLocal/python/DBGCVectors/DBGCVectors.xlsx
+++ b/demoForLocal/python/DBGCVectors/DBGCVectors.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <s:workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:s="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <s:workbookPr codeName="ThisWorkbook"/>
+  <s:workbookPr/>
   <s:bookViews>
     <s:workbookView activeTab="0"/>
   </s:bookViews>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="177">
   <si>
     <t>ID</t>
   </si>
@@ -544,13 +544,7 @@
     <t>ReferenceEnergy</t>
   </si>
   <si>
-    <t>test1</t>
-  </si>
-  <si>
-    <t>test2</t>
-  </si>
-  <si>
-    <t>test3</t>
+    <t>testmole</t>
   </si>
 </sst>
 </file>
@@ -887,7 +881,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:FW6"/>
+  <dimension ref="A1:FW4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -911,7 +905,7 @@
     </row>
     <row r="2" spans="1:179">
       <c r="B2" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D2" t="n">
         <v>170</v>
@@ -1950,7 +1944,7 @@
         <v>1</v>
       </c>
       <c r="F4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G4" t="n">
         <v>0</v>
@@ -1965,31 +1959,31 @@
         <v>0</v>
       </c>
       <c r="K4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N4" t="n">
         <v>0</v>
       </c>
       <c r="O4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P4" t="n">
         <v>0</v>
       </c>
       <c r="Q4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R4" t="n">
         <v>0</v>
       </c>
       <c r="S4" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="T4" t="n">
         <v>0</v>
@@ -2016,13 +2010,13 @@
         <v>0</v>
       </c>
       <c r="AB4" t="n">
-        <v>0</v>
+        <v>7.582560427911907e-10</v>
       </c>
       <c r="AC4" t="n">
-        <v>0</v>
+        <v>0.002478752176666358</v>
       </c>
       <c r="AD4" t="n">
-        <v>0</v>
+        <v>0.04978706836786394</v>
       </c>
       <c r="AE4" t="n">
         <v>0</v>
@@ -2040,7 +2034,7 @@
         <v>0</v>
       </c>
       <c r="AJ4" t="n">
-        <v>0</v>
+        <v>0.05239569569327056</v>
       </c>
       <c r="AK4" t="n">
         <v>0</v>
@@ -2226,31 +2220,31 @@
         <v>0</v>
       </c>
       <c r="CT4" t="n">
-        <v>0.0001234098040866796</v>
+        <v>0</v>
       </c>
       <c r="CU4" t="n">
-        <v>0</v>
+        <v>1.879528816539083e-12</v>
       </c>
       <c r="CV4" t="n">
-        <v>0</v>
+        <v>3.775134544279098e-11</v>
       </c>
       <c r="CW4" t="n">
         <v>0</v>
       </c>
       <c r="CX4" t="n">
-        <v>0.002602161980753038</v>
+        <v>0</v>
       </c>
       <c r="CY4" t="n">
         <v>0</v>
       </c>
       <c r="CZ4" t="n">
-        <v>0.0522658205445303</v>
+        <v>0</v>
       </c>
       <c r="DA4" t="n">
         <v>0</v>
       </c>
       <c r="DB4" t="n">
-        <v>0.0522658205445303</v>
+        <v>0.05239569569327055</v>
       </c>
       <c r="DC4" t="n">
         <v>0</v>
@@ -2265,7 +2259,7 @@
         <v>0</v>
       </c>
       <c r="DG4" t="n">
-        <v>0</v>
+        <v>0.04978706836786394</v>
       </c>
       <c r="DH4" t="n">
         <v>0</v>
@@ -2283,7 +2277,7 @@
         <v>0</v>
       </c>
       <c r="DM4" t="n">
-        <v>0</v>
+        <v>0.0001298759447476425</v>
       </c>
       <c r="DN4" t="n">
         <v>0</v>
@@ -2313,7 +2307,7 @@
         <v>0</v>
       </c>
       <c r="DW4" t="n">
-        <v>0</v>
+        <v>0.002608628083662656</v>
       </c>
       <c r="DX4" t="n">
         <v>0</v>
@@ -2358,13 +2352,13 @@
         <v>0</v>
       </c>
       <c r="EL4" t="n">
-        <v>0.04978706836786394</v>
+        <v>0</v>
       </c>
       <c r="EM4" t="n">
         <v>0</v>
       </c>
       <c r="EN4" t="n">
-        <v>0.002478752176666358</v>
+        <v>0</v>
       </c>
       <c r="EO4" t="n">
         <v>0</v>
@@ -2403,7 +2397,7 @@
         <v>0</v>
       </c>
       <c r="FA4" t="n">
-        <v>0.04978706836786394</v>
+        <v>0</v>
       </c>
       <c r="FB4" t="n">
         <v>0</v>
@@ -2430,7 +2424,7 @@
         <v>0</v>
       </c>
       <c r="FJ4" t="n">
-        <v>0</v>
+        <v>0.2592331742852723</v>
       </c>
       <c r="FK4" t="n">
         <v>0</v>
@@ -2461,1042 +2455,6 @@
       </c>
       <c r="FV4" t="s">
         <v>176</v>
-      </c>
-    </row>
-    <row r="5" spans="1:179">
-      <c r="A5" t="n">
-        <v>2</v>
-      </c>
-      <c r="F5" t="n">
-        <v>0</v>
-      </c>
-      <c r="G5" t="n">
-        <v>0</v>
-      </c>
-      <c r="H5" t="n">
-        <v>0</v>
-      </c>
-      <c r="I5" t="n">
-        <v>2</v>
-      </c>
-      <c r="J5" t="n">
-        <v>1</v>
-      </c>
-      <c r="K5" t="n">
-        <v>3</v>
-      </c>
-      <c r="L5" t="n">
-        <v>0</v>
-      </c>
-      <c r="M5" t="n">
-        <v>0</v>
-      </c>
-      <c r="N5" t="n">
-        <v>0</v>
-      </c>
-      <c r="O5" t="n">
-        <v>0</v>
-      </c>
-      <c r="P5" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q5" t="n">
-        <v>0</v>
-      </c>
-      <c r="R5" t="n">
-        <v>0</v>
-      </c>
-      <c r="S5" t="n">
-        <v>1</v>
-      </c>
-      <c r="T5" t="n">
-        <v>0</v>
-      </c>
-      <c r="U5" t="n">
-        <v>2</v>
-      </c>
-      <c r="V5" t="n">
-        <v>0</v>
-      </c>
-      <c r="W5" t="n">
-        <v>0</v>
-      </c>
-      <c r="X5" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y5" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z5" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA5" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB5" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC5" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD5" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE5" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF5" t="n">
-        <v>0</v>
-      </c>
-      <c r="AG5" t="n">
-        <v>0</v>
-      </c>
-      <c r="AH5" t="n">
-        <v>0</v>
-      </c>
-      <c r="AI5" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ5" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK5" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL5" t="n">
-        <v>0</v>
-      </c>
-      <c r="AM5" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN5" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO5" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP5" t="n">
-        <v>0</v>
-      </c>
-      <c r="AQ5" t="n">
-        <v>0</v>
-      </c>
-      <c r="AR5" t="n">
-        <v>0</v>
-      </c>
-      <c r="AS5" t="n">
-        <v>0</v>
-      </c>
-      <c r="AT5" t="n">
-        <v>0</v>
-      </c>
-      <c r="AU5" t="n">
-        <v>0</v>
-      </c>
-      <c r="AV5" t="n">
-        <v>0</v>
-      </c>
-      <c r="AW5" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX5" t="n">
-        <v>0</v>
-      </c>
-      <c r="AY5" t="n">
-        <v>0</v>
-      </c>
-      <c r="AZ5" t="n">
-        <v>0</v>
-      </c>
-      <c r="BA5" t="n">
-        <v>0</v>
-      </c>
-      <c r="BB5" t="n">
-        <v>0</v>
-      </c>
-      <c r="BC5" t="n">
-        <v>0</v>
-      </c>
-      <c r="BD5" t="n">
-        <v>0</v>
-      </c>
-      <c r="BE5" t="n">
-        <v>0</v>
-      </c>
-      <c r="BF5" t="n">
-        <v>0</v>
-      </c>
-      <c r="BG5" t="n">
-        <v>0</v>
-      </c>
-      <c r="BH5" t="n">
-        <v>0</v>
-      </c>
-      <c r="BI5" t="n">
-        <v>0</v>
-      </c>
-      <c r="BJ5" t="n">
-        <v>0</v>
-      </c>
-      <c r="BK5" t="n">
-        <v>0</v>
-      </c>
-      <c r="BL5" t="n">
-        <v>0</v>
-      </c>
-      <c r="BM5" t="n">
-        <v>0</v>
-      </c>
-      <c r="BN5" t="n">
-        <v>0</v>
-      </c>
-      <c r="BO5" t="n">
-        <v>0</v>
-      </c>
-      <c r="BP5" t="n">
-        <v>0</v>
-      </c>
-      <c r="BQ5" t="n">
-        <v>0</v>
-      </c>
-      <c r="BR5" t="n">
-        <v>0</v>
-      </c>
-      <c r="BS5" t="n">
-        <v>0.04978706836786394</v>
-      </c>
-      <c r="BT5" t="n">
-        <v>0.0001295540164400078</v>
-      </c>
-      <c r="BU5" t="n">
-        <v>0.005333877977946084</v>
-      </c>
-      <c r="BV5" t="n">
-        <v>0</v>
-      </c>
-      <c r="BW5" t="n">
-        <v>0</v>
-      </c>
-      <c r="BX5" t="n">
-        <v>0</v>
-      </c>
-      <c r="BY5" t="n">
-        <v>0</v>
-      </c>
-      <c r="BZ5" t="n">
-        <v>0</v>
-      </c>
-      <c r="CA5" t="n">
-        <v>0</v>
-      </c>
-      <c r="CB5" t="n">
-        <v>0</v>
-      </c>
-      <c r="CC5" t="n">
-        <v>0.0522658205445303</v>
-      </c>
-      <c r="CD5" t="n">
-        <v>0</v>
-      </c>
-      <c r="CE5" t="n">
-        <v>0.05486798252528334</v>
-      </c>
-      <c r="CF5" t="n">
-        <v>0</v>
-      </c>
-      <c r="CG5" t="n">
-        <v>0</v>
-      </c>
-      <c r="CH5" t="n">
-        <v>0.002602177210732783</v>
-      </c>
-      <c r="CI5" t="n">
-        <v>0</v>
-      </c>
-      <c r="CJ5" t="n">
-        <v>0</v>
-      </c>
-      <c r="CK5" t="n">
-        <v>0</v>
-      </c>
-      <c r="CL5" t="n">
-        <v>0</v>
-      </c>
-      <c r="CM5" t="n">
-        <v>0</v>
-      </c>
-      <c r="CN5" t="n">
-        <v>0</v>
-      </c>
-      <c r="CO5" t="n">
-        <v>0</v>
-      </c>
-      <c r="CP5" t="n">
-        <v>3.059023205018258e-07</v>
-      </c>
-      <c r="CQ5" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR5" t="n">
-        <v>0.0522658205445303</v>
-      </c>
-      <c r="CS5" t="n">
-        <v>0</v>
-      </c>
-      <c r="CT5" t="n">
-        <v>0.0001237309363869261</v>
-      </c>
-      <c r="CU5" t="n">
-        <v>0</v>
-      </c>
-      <c r="CV5" t="n">
-        <v>0</v>
-      </c>
-      <c r="CW5" t="n">
-        <v>0</v>
-      </c>
-      <c r="CX5" t="n">
-        <v>0</v>
-      </c>
-      <c r="CY5" t="n">
-        <v>0</v>
-      </c>
-      <c r="CZ5" t="n">
-        <v>0</v>
-      </c>
-      <c r="DA5" t="n">
-        <v>0</v>
-      </c>
-      <c r="DB5" t="n">
-        <v>0.04979351848253778</v>
-      </c>
-      <c r="DC5" t="n">
-        <v>0</v>
-      </c>
-      <c r="DD5" t="n">
-        <v>0.1045380912037344</v>
-      </c>
-      <c r="DE5" t="n">
-        <v>0</v>
-      </c>
-      <c r="DF5" t="n">
-        <v>0</v>
-      </c>
-      <c r="DG5" t="n">
-        <v>0</v>
-      </c>
-      <c r="DH5" t="n">
-        <v>0</v>
-      </c>
-      <c r="DI5" t="n">
-        <v>0</v>
-      </c>
-      <c r="DJ5" t="n">
-        <v>0</v>
-      </c>
-      <c r="DK5" t="n">
-        <v>0</v>
-      </c>
-      <c r="DL5" t="n">
-        <v>0</v>
-      </c>
-      <c r="DM5" t="n">
-        <v>0</v>
-      </c>
-      <c r="DN5" t="n">
-        <v>0</v>
-      </c>
-      <c r="DO5" t="n">
-        <v>0</v>
-      </c>
-      <c r="DP5" t="n">
-        <v>0</v>
-      </c>
-      <c r="DQ5" t="n">
-        <v>0</v>
-      </c>
-      <c r="DR5" t="n">
-        <v>0</v>
-      </c>
-      <c r="DS5" t="n">
-        <v>0</v>
-      </c>
-      <c r="DT5" t="n">
-        <v>0</v>
-      </c>
-      <c r="DU5" t="n">
-        <v>0</v>
-      </c>
-      <c r="DV5" t="n">
-        <v>0</v>
-      </c>
-      <c r="DW5" t="n">
-        <v>0</v>
-      </c>
-      <c r="DX5" t="n">
-        <v>0</v>
-      </c>
-      <c r="DY5" t="n">
-        <v>0</v>
-      </c>
-      <c r="DZ5" t="n">
-        <v>0</v>
-      </c>
-      <c r="EA5" t="n">
-        <v>0</v>
-      </c>
-      <c r="EB5" t="n">
-        <v>0</v>
-      </c>
-      <c r="EC5" t="n">
-        <v>0</v>
-      </c>
-      <c r="ED5" t="n">
-        <v>0</v>
-      </c>
-      <c r="EE5" t="n">
-        <v>0</v>
-      </c>
-      <c r="EF5" t="n">
-        <v>0</v>
-      </c>
-      <c r="EG5" t="n">
-        <v>0</v>
-      </c>
-      <c r="EH5" t="n">
-        <v>0</v>
-      </c>
-      <c r="EI5" t="n">
-        <v>0</v>
-      </c>
-      <c r="EJ5" t="n">
-        <v>0</v>
-      </c>
-      <c r="EK5" t="n">
-        <v>0</v>
-      </c>
-      <c r="EL5" t="n">
-        <v>0</v>
-      </c>
-      <c r="EM5" t="n">
-        <v>0</v>
-      </c>
-      <c r="EN5" t="n">
-        <v>0</v>
-      </c>
-      <c r="EO5" t="n">
-        <v>0</v>
-      </c>
-      <c r="EP5" t="n">
-        <v>0</v>
-      </c>
-      <c r="EQ5" t="n">
-        <v>0</v>
-      </c>
-      <c r="ER5" t="n">
-        <v>0</v>
-      </c>
-      <c r="ES5" t="n">
-        <v>0</v>
-      </c>
-      <c r="ET5" t="n">
-        <v>0</v>
-      </c>
-      <c r="EU5" t="n">
-        <v>0</v>
-      </c>
-      <c r="EV5" t="n">
-        <v>0</v>
-      </c>
-      <c r="EW5" t="n">
-        <v>0</v>
-      </c>
-      <c r="EX5" t="n">
-        <v>0</v>
-      </c>
-      <c r="EY5" t="n">
-        <v>0</v>
-      </c>
-      <c r="EZ5" t="n">
-        <v>0</v>
-      </c>
-      <c r="FA5" t="n">
-        <v>0</v>
-      </c>
-      <c r="FB5" t="n">
-        <v>0</v>
-      </c>
-      <c r="FC5" t="n">
-        <v>0</v>
-      </c>
-      <c r="FD5" t="n">
-        <v>0</v>
-      </c>
-      <c r="FE5" t="n">
-        <v>0</v>
-      </c>
-      <c r="FF5" t="n">
-        <v>0</v>
-      </c>
-      <c r="FG5" t="n">
-        <v>0</v>
-      </c>
-      <c r="FH5" t="n">
-        <v>0</v>
-      </c>
-      <c r="FI5" t="n">
-        <v>0</v>
-      </c>
-      <c r="FJ5" t="n">
-        <v>0</v>
-      </c>
-      <c r="FK5" t="n">
-        <v>0</v>
-      </c>
-      <c r="FL5" t="n">
-        <v>0.0001295540164400078</v>
-      </c>
-      <c r="FM5" t="n">
-        <v>0</v>
-      </c>
-      <c r="FN5" t="n">
-        <v>0</v>
-      </c>
-      <c r="FO5" t="n">
-        <v>0</v>
-      </c>
-      <c r="FP5" t="n">
-        <v>0</v>
-      </c>
-      <c r="FQ5" t="n">
-        <v>0.04978706836786394</v>
-      </c>
-      <c r="FR5" t="n">
-        <v>0</v>
-      </c>
-      <c r="FS5" t="n">
-        <v>0</v>
-      </c>
-      <c r="FV5" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="6" spans="1:179">
-      <c r="A6" t="n">
-        <v>3</v>
-      </c>
-      <c r="F6" t="n">
-        <v>0</v>
-      </c>
-      <c r="G6" t="n">
-        <v>0</v>
-      </c>
-      <c r="H6" t="n">
-        <v>0</v>
-      </c>
-      <c r="I6" t="n">
-        <v>0</v>
-      </c>
-      <c r="J6" t="n">
-        <v>0</v>
-      </c>
-      <c r="K6" t="n">
-        <v>5</v>
-      </c>
-      <c r="L6" t="n">
-        <v>0</v>
-      </c>
-      <c r="M6" t="n">
-        <v>0</v>
-      </c>
-      <c r="N6" t="n">
-        <v>0</v>
-      </c>
-      <c r="O6" t="n">
-        <v>0</v>
-      </c>
-      <c r="P6" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q6" t="n">
-        <v>0</v>
-      </c>
-      <c r="R6" t="n">
-        <v>1</v>
-      </c>
-      <c r="S6" t="n">
-        <v>2</v>
-      </c>
-      <c r="T6" t="n">
-        <v>0</v>
-      </c>
-      <c r="U6" t="n">
-        <v>1</v>
-      </c>
-      <c r="V6" t="n">
-        <v>1</v>
-      </c>
-      <c r="W6" t="n">
-        <v>0</v>
-      </c>
-      <c r="X6" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y6" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z6" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA6" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB6" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC6" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD6" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE6" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF6" t="n">
-        <v>0</v>
-      </c>
-      <c r="AG6" t="n">
-        <v>0</v>
-      </c>
-      <c r="AH6" t="n">
-        <v>0</v>
-      </c>
-      <c r="AI6" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ6" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK6" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL6" t="n">
-        <v>0</v>
-      </c>
-      <c r="AM6" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN6" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO6" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP6" t="n">
-        <v>0</v>
-      </c>
-      <c r="AQ6" t="n">
-        <v>0</v>
-      </c>
-      <c r="AR6" t="n">
-        <v>0</v>
-      </c>
-      <c r="AS6" t="n">
-        <v>0</v>
-      </c>
-      <c r="AT6" t="n">
-        <v>0</v>
-      </c>
-      <c r="AU6" t="n">
-        <v>0</v>
-      </c>
-      <c r="AV6" t="n">
-        <v>0</v>
-      </c>
-      <c r="AW6" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX6" t="n">
-        <v>0</v>
-      </c>
-      <c r="AY6" t="n">
-        <v>0</v>
-      </c>
-      <c r="AZ6" t="n">
-        <v>0</v>
-      </c>
-      <c r="BA6" t="n">
-        <v>0</v>
-      </c>
-      <c r="BB6" t="n">
-        <v>0</v>
-      </c>
-      <c r="BC6" t="n">
-        <v>0</v>
-      </c>
-      <c r="BD6" t="n">
-        <v>0</v>
-      </c>
-      <c r="BE6" t="n">
-        <v>0</v>
-      </c>
-      <c r="BF6" t="n">
-        <v>0</v>
-      </c>
-      <c r="BG6" t="n">
-        <v>0</v>
-      </c>
-      <c r="BH6" t="n">
-        <v>0</v>
-      </c>
-      <c r="BI6" t="n">
-        <v>0</v>
-      </c>
-      <c r="BJ6" t="n">
-        <v>0</v>
-      </c>
-      <c r="BK6" t="n">
-        <v>0</v>
-      </c>
-      <c r="BL6" t="n">
-        <v>0</v>
-      </c>
-      <c r="BM6" t="n">
-        <v>0</v>
-      </c>
-      <c r="BN6" t="n">
-        <v>0</v>
-      </c>
-      <c r="BO6" t="n">
-        <v>0</v>
-      </c>
-      <c r="BP6" t="n">
-        <v>0</v>
-      </c>
-      <c r="BQ6" t="n">
-        <v>0</v>
-      </c>
-      <c r="BR6" t="n">
-        <v>0</v>
-      </c>
-      <c r="BS6" t="n">
-        <v>0</v>
-      </c>
-      <c r="BT6" t="n">
-        <v>0</v>
-      </c>
-      <c r="BU6" t="n">
-        <v>0</v>
-      </c>
-      <c r="BV6" t="n">
-        <v>0</v>
-      </c>
-      <c r="BW6" t="n">
-        <v>0</v>
-      </c>
-      <c r="BX6" t="n">
-        <v>0</v>
-      </c>
-      <c r="BY6" t="n">
-        <v>0</v>
-      </c>
-      <c r="BZ6" t="n">
-        <v>0</v>
-      </c>
-      <c r="CA6" t="n">
-        <v>0</v>
-      </c>
-      <c r="CB6" t="n">
-        <v>0</v>
-      </c>
-      <c r="CC6" t="n">
-        <v>0</v>
-      </c>
-      <c r="CD6" t="n">
-        <v>0</v>
-      </c>
-      <c r="CE6" t="n">
-        <v>0</v>
-      </c>
-      <c r="CF6" t="n">
-        <v>0</v>
-      </c>
-      <c r="CG6" t="n">
-        <v>0</v>
-      </c>
-      <c r="CH6" t="n">
-        <v>0</v>
-      </c>
-      <c r="CI6" t="n">
-        <v>0</v>
-      </c>
-      <c r="CJ6" t="n">
-        <v>0</v>
-      </c>
-      <c r="CK6" t="n">
-        <v>0</v>
-      </c>
-      <c r="CL6" t="n">
-        <v>0</v>
-      </c>
-      <c r="CM6" t="n">
-        <v>0</v>
-      </c>
-      <c r="CN6" t="n">
-        <v>0</v>
-      </c>
-      <c r="CO6" t="n">
-        <v>0</v>
-      </c>
-      <c r="CP6" t="n">
-        <v>0</v>
-      </c>
-      <c r="CQ6" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR6" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS6" t="n">
-        <v>0</v>
-      </c>
-      <c r="CT6" t="n">
-        <v>0.007444236156275415</v>
-      </c>
-      <c r="CU6" t="n">
-        <v>0</v>
-      </c>
-      <c r="CV6" t="n">
-        <v>0</v>
-      </c>
-      <c r="CW6" t="n">
-        <v>0</v>
-      </c>
-      <c r="CX6" t="n">
-        <v>0</v>
-      </c>
-      <c r="CY6" t="n">
-        <v>0</v>
-      </c>
-      <c r="CZ6" t="n">
-        <v>0</v>
-      </c>
-      <c r="DA6" t="n">
-        <v>0.04992891080901061</v>
-      </c>
-      <c r="DB6" t="n">
-        <v>0.05761198694718303</v>
-      </c>
-      <c r="DC6" t="n">
-        <v>0</v>
-      </c>
-      <c r="DD6" t="n">
-        <v>0.005327733765592756</v>
-      </c>
-      <c r="DE6" t="n">
-        <v>0.1493734935282985</v>
-      </c>
-      <c r="DF6" t="n">
-        <v>0</v>
-      </c>
-      <c r="DG6" t="n">
-        <v>0</v>
-      </c>
-      <c r="DH6" t="n">
-        <v>0</v>
-      </c>
-      <c r="DI6" t="n">
-        <v>0</v>
-      </c>
-      <c r="DJ6" t="n">
-        <v>0</v>
-      </c>
-      <c r="DK6" t="n">
-        <v>0</v>
-      </c>
-      <c r="DL6" t="n">
-        <v>0</v>
-      </c>
-      <c r="DM6" t="n">
-        <v>0</v>
-      </c>
-      <c r="DN6" t="n">
-        <v>0</v>
-      </c>
-      <c r="DO6" t="n">
-        <v>0</v>
-      </c>
-      <c r="DP6" t="n">
-        <v>0</v>
-      </c>
-      <c r="DQ6" t="n">
-        <v>0</v>
-      </c>
-      <c r="DR6" t="n">
-        <v>0</v>
-      </c>
-      <c r="DS6" t="n">
-        <v>0</v>
-      </c>
-      <c r="DT6" t="n">
-        <v>0</v>
-      </c>
-      <c r="DU6" t="n">
-        <v>0</v>
-      </c>
-      <c r="DV6" t="n">
-        <v>0</v>
-      </c>
-      <c r="DW6" t="n">
-        <v>0</v>
-      </c>
-      <c r="DX6" t="n">
-        <v>0</v>
-      </c>
-      <c r="DY6" t="n">
-        <v>0</v>
-      </c>
-      <c r="DZ6" t="n">
-        <v>0</v>
-      </c>
-      <c r="EA6" t="n">
-        <v>0</v>
-      </c>
-      <c r="EB6" t="n">
-        <v>0</v>
-      </c>
-      <c r="EC6" t="n">
-        <v>0</v>
-      </c>
-      <c r="ED6" t="n">
-        <v>0</v>
-      </c>
-      <c r="EE6" t="n">
-        <v>0</v>
-      </c>
-      <c r="EF6" t="n">
-        <v>0</v>
-      </c>
-      <c r="EG6" t="n">
-        <v>0</v>
-      </c>
-      <c r="EH6" t="n">
-        <v>0</v>
-      </c>
-      <c r="EI6" t="n">
-        <v>0</v>
-      </c>
-      <c r="EJ6" t="n">
-        <v>0</v>
-      </c>
-      <c r="EK6" t="n">
-        <v>0</v>
-      </c>
-      <c r="EL6" t="n">
-        <v>0</v>
-      </c>
-      <c r="EM6" t="n">
-        <v>0</v>
-      </c>
-      <c r="EN6" t="n">
-        <v>0</v>
-      </c>
-      <c r="EO6" t="n">
-        <v>0</v>
-      </c>
-      <c r="EP6" t="n">
-        <v>0</v>
-      </c>
-      <c r="EQ6" t="n">
-        <v>0</v>
-      </c>
-      <c r="ER6" t="n">
-        <v>0</v>
-      </c>
-      <c r="ES6" t="n">
-        <v>0</v>
-      </c>
-      <c r="ET6" t="n">
-        <v>0</v>
-      </c>
-      <c r="EU6" t="n">
-        <v>0</v>
-      </c>
-      <c r="EV6" t="n">
-        <v>0</v>
-      </c>
-      <c r="EW6" t="n">
-        <v>0</v>
-      </c>
-      <c r="EX6" t="n">
-        <v>0</v>
-      </c>
-      <c r="EY6" t="n">
-        <v>0</v>
-      </c>
-      <c r="EZ6" t="n">
-        <v>0</v>
-      </c>
-      <c r="FA6" t="n">
-        <v>0</v>
-      </c>
-      <c r="FB6" t="n">
-        <v>0</v>
-      </c>
-      <c r="FC6" t="n">
-        <v>0</v>
-      </c>
-      <c r="FD6" t="n">
-        <v>0</v>
-      </c>
-      <c r="FE6" t="n">
-        <v>0</v>
-      </c>
-      <c r="FF6" t="n">
-        <v>0.004957504353332717</v>
-      </c>
-      <c r="FG6" t="n">
-        <v>0</v>
-      </c>
-      <c r="FH6" t="n">
-        <v>0.04978706836786394</v>
-      </c>
-      <c r="FI6" t="n">
-        <v>0.0001234098040866796</v>
-      </c>
-      <c r="FJ6" t="n">
-        <v>0.002478752176666358</v>
-      </c>
-      <c r="FK6" t="n">
-        <v>0</v>
-      </c>
-      <c r="FL6" t="n">
-        <v>0.09957413673572789</v>
-      </c>
-      <c r="FM6" t="n">
-        <v>0.04991047817195062</v>
-      </c>
-      <c r="FN6" t="n">
-        <v>0</v>
-      </c>
-      <c r="FO6" t="n">
-        <v>0</v>
-      </c>
-      <c r="FP6" t="n">
-        <v>0</v>
-      </c>
-      <c r="FQ6" t="n">
-        <v>0</v>
-      </c>
-      <c r="FR6" t="n">
-        <v>0.002478752176666358</v>
-      </c>
-      <c r="FS6" t="n">
-        <v>0</v>
-      </c>
-      <c r="FV6" t="s">
-        <v>178</v>
       </c>
     </row>
   </sheetData>

</xml_diff>